<commit_message>
Ajuste no readme e atualização do histórico de treinamentos
</commit_message>
<xml_diff>
--- a/Registro de treinamentos.xlsx
+++ b/Registro de treinamentos.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Redes com embeddings sem pré-treino" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Redes com embedding pré-treinado NILC" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Redes com embedding pré-treinado acórdãos" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="58">
   <si>
     <t xml:space="preserve">Melhor val_cat_acc</t>
   </si>
@@ -117,6 +118,15 @@
   </si>
   <si>
     <t xml:space="preserve">Regressão Logística</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipamento utilizado:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Core i5-7400 3GHz x 4 núcleos; memória 16 GB; GPU GeForce GTX 1070 (1920 núcleos, 8 GB VRAM); HD 1 TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema operacional 64 bits Ubuntu 18.04.3 LTS, GNOME 3.28.2</t>
   </si>
   <si>
     <t xml:space="preserve">Embedding treinada fixa + densa 2048 + 1024 + dropout .6</t>
@@ -192,16 +202,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,70 +231,18 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -290,9 +250,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,54 +262,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -356,23 +275,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,42 +300,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,78 +330,69 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -526,7 +404,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -542,7 +420,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -569,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,15 +1018,44 @@
       <c r="A35" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="5" t="n">
-        <v>0.87</v>
-      </c>
+      <c r="E35" s="12" t="n">
+        <v>0.867</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D30:F30"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1165,15 +1072,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ34"/>
+  <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="79.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="79.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.96"/>
@@ -1214,7 +1121,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -1238,7 +1145,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
@@ -1262,7 +1169,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
@@ -1286,7 +1193,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>9</v>
@@ -1310,7 +1217,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>9</v>
@@ -1321,7 +1228,7 @@
       <c r="D7" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E7" s="12" t="n">
+      <c r="E7" s="14" t="n">
         <v>0.6748</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -1334,7 +1241,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
@@ -1358,7 +1265,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>26</v>
@@ -1382,7 +1289,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
@@ -1406,7 +1313,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>26</v>
@@ -1430,7 +1337,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>26</v>
@@ -1441,7 +1348,7 @@
       <c r="D12" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E12" s="15" t="n">
         <v>0.8573</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -1454,7 +1361,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>26</v>
@@ -1478,7 +1385,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>26</v>
@@ -1489,7 +1396,7 @@
       <c r="D14" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E14" s="13" t="n">
+      <c r="E14" s="15" t="n">
         <v>0.8532</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -1502,7 +1409,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>26</v>
@@ -1513,7 +1420,7 @@
       <c r="D15" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E15" s="13" t="n">
+      <c r="E15" s="15" t="n">
         <v>0.8547</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -1526,7 +1433,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>26</v>
@@ -1550,7 +1457,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>26</v>
@@ -1574,7 +1481,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>26</v>
@@ -1585,7 +1492,7 @@
       <c r="D18" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="15" t="n">
         <v>0.8554</v>
       </c>
       <c r="F18" s="0" t="n">
@@ -1598,7 +1505,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>26</v>
@@ -1622,7 +1529,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>26</v>
@@ -1646,7 +1553,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>26</v>
@@ -1657,7 +1564,7 @@
       <c r="D21" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="15" t="n">
         <v>0.8573</v>
       </c>
       <c r="F21" s="0" t="n">
@@ -1670,7 +1577,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>26</v>
@@ -1681,7 +1588,7 @@
       <c r="D22" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E22" s="14" t="n">
+      <c r="E22" s="16" t="n">
         <v>0.8603</v>
       </c>
       <c r="F22" s="0" t="n">
@@ -1694,7 +1601,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>26</v>
@@ -1705,7 +1612,7 @@
       <c r="D23" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E23" s="14" t="n">
+      <c r="E23" s="16" t="n">
         <v>0.8629</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -1718,7 +1625,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>13</v>
@@ -1742,7 +1649,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>9</v>
@@ -1766,7 +1673,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>26</v>
@@ -1790,7 +1697,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>26</v>
@@ -1801,7 +1708,7 @@
       <c r="D27" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E27" s="13" t="n">
+      <c r="E27" s="15" t="n">
         <v>0.8584</v>
       </c>
       <c r="F27" s="0" t="n">
@@ -1856,22 +1763,796 @@
       <c r="A34" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="5" t="n">
-        <v>0.87</v>
-      </c>
+      <c r="E34" s="12" t="n">
+        <v>0.867</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="79.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.7075</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <f aca="false">TIME( , ,F3*C3)</f>
+        <v>0.00393518518518518</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.6962</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <f aca="false">TIME( , ,F4*C4)</f>
+        <v>0.00393518518518518</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.7007</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <f aca="false">TIME( , ,F5*C5)</f>
+        <v>0.0037037037037037</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.7112</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <f aca="false">TIME( , ,F6*C6)</f>
+        <v>0.00416666666666667</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>0.6921</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">TIME( , ,F7*C7)</f>
+        <v>0.00416666666666667</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.694</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <f aca="false">TIME( , ,F8*C8)</f>
+        <v>0.00416666666666667</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <f aca="false">TIME( , ,F9*C9)</f>
+        <v>0.0122685185185185</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" s="16" t="n">
+        <v>0.8607</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <f aca="false">TIME( , ,F10*C10)</f>
+        <v>0.0131944444444444</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <f aca="false">TIME( , ,F11*C11)</f>
+        <v>0.00532407407407407</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" s="15" t="n">
+        <v>0.8543</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <f aca="false">TIME( , ,F12*C12)</f>
+        <v>0.0168981481481482</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.6782</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <f aca="false">TIME( , ,F13*C13)</f>
+        <v>0.00833333333333333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" s="16" t="n">
+        <v>0.8629</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <f aca="false">TIME( , ,F14*C14)</f>
+        <v>0.0233796296296296</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E15" s="15" t="n">
+        <v>0.8569</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <f aca="false">TIME( , ,F15*C15)</f>
+        <v>0.0287037037037037</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E16" s="15" t="n">
+        <v>0.8581</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <f aca="false">TIME( , ,F16*C16)</f>
+        <v>0.0127314814814815</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0.8359</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <f aca="false">TIME( , ,F17*C17)</f>
+        <v>0.0127314814814815</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E18" s="15" t="n">
+        <v>0.8581</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <f aca="false">TIME( , ,F18*C18)</f>
+        <v>0.012962962962963</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E19" s="16" t="n">
+        <v>0.8618</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <f aca="false">TIME( , ,F19*C19)</f>
+        <v>0.012962962962963</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E20" s="15" t="n">
+        <v>0.8577</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <f aca="false">TIME( , ,F20*C20)</f>
+        <v>0.0131944444444444</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E21" s="15" t="n">
+        <v>0.8588</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <f aca="false">TIME( , ,F21*C21)</f>
+        <v>0.0131944444444444</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <v>0.8697</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <f aca="false">TIME( , ,F22*C22)</f>
+        <v>0.0148148148148148</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E23" s="16" t="n">
+        <v>0.8693</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G23" s="6" t="n">
+        <f aca="false">TIME( , ,F23*C23)</f>
+        <v>0.0148148148148148</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E24" s="16" t="n">
+        <v>0.8611</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="G24" s="6" t="n">
+        <f aca="false">TIME( , ,F24*C24)</f>
+        <v>0.012962962962963</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E25" s="15" t="n">
+        <v>0.8539</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <f aca="false">TIME( , ,F25*C25)</f>
+        <v>0.012962962962963</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E26" s="16" t="n">
+        <v>0.8611</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <f aca="false">TIME( , ,F26*C26)</f>
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E27" s="16" t="n">
+        <v>0.8689</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <f aca="false">TIME( , ,F27*C27)</f>
+        <v>0.0148148148148148</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E28" s="15" t="n">
+        <v>0.8535</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <f aca="false">TIME( , ,F28*C28)</f>
+        <v>0.00648148148148148</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="6" t="n">
+        <f aca="false">SUM(G3:G28)</f>
+        <v>0.311805555555556</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="12" t="n">
+        <v>0.867</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>